<commit_message>
Seleção de Arquivos Check-In
</commit_message>
<xml_diff>
--- a/data/check-in.xlsx
+++ b/data/check-in.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMO" sheetId="1" state="visible" r:id="rId3"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="56">
   <si>
     <t xml:space="preserve">Autor: Miguel Souza Cardeal</t>
   </si>
@@ -511,6 +511,9 @@
       </rPr>
       <t xml:space="preserve">13</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ALALALALA</t>
   </si>
   <si>
     <r>
@@ -1325,7 +1328,7 @@
   </sheetPr>
   <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -1990,11 +1993,11 @@
       <c r="K27" s="13"/>
       <c r="L27" s="14" t="n">
         <f aca="false">Ago!C7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="15" t="n">
         <f aca="false">IFERROR(L27/$E$9,"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,11 +2022,11 @@
       <c r="K28" s="13"/>
       <c r="L28" s="14" t="n">
         <f aca="false">Ago!C8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" s="15" t="n">
         <f aca="false">IFERROR(L28/$E$9,"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,11 +2037,11 @@
       <c r="D29" s="13"/>
       <c r="E29" s="14" t="n">
         <f aca="false">Jul!F7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="15" t="n">
         <f aca="false">IFERROR(E29/$E$9,"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="13" t="s">
@@ -3223,7 +3226,7 @@
   <dimension ref="B1:S203"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3257,7 +3260,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -3347,7 +3350,7 @@
       </c>
       <c r="C7" s="14" t="n">
         <f aca="false">COUNT(B:B)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>34</v>
@@ -3362,7 +3365,7 @@
       </c>
       <c r="I7" s="14" t="n">
         <f aca="false">COUNTIF(I:I,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -3375,14 +3378,14 @@
       </c>
       <c r="C8" s="14" t="n">
         <f aca="false">COUNT(D:D)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="14" t="n">
         <f aca="false">COUNTIF(H:H,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -3454,30 +3457,16 @@
       <c r="N12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="22" t="n">
-        <v>45722</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="23" t="n">
-        <v>5551999142035</v>
-      </c>
-      <c r="E13" s="23" t="n">
-        <v>215</v>
-      </c>
-      <c r="F13" s="22" t="n">
-        <v>45723</v>
-      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -6425,7 +6414,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -9593,7 +9582,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -12761,7 +12750,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -15929,7 +15918,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -19117,8 +19106,8 @@
   </sheetPr>
   <dimension ref="B1:S203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38108,7 +38097,7 @@
   <dimension ref="B1:S203"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38239,7 +38228,7 @@
       </c>
       <c r="F7" s="14" t="n">
         <f aca="false">COUNTIF(G:G,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="13" t="s">
@@ -38267,7 +38256,7 @@
       </c>
       <c r="F8" s="14" t="n">
         <f aca="false">COUNTIF(H:H,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -38337,10 +38326,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="n">
-        <v>45722</v>
+        <v>45725</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D13" s="23" t="n">
         <v>5551999142035</v>
@@ -38352,10 +38341,10 @@
         <v>45723</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Classe JanelaEnvio e formulação do método de envio em massa
</commit_message>
<xml_diff>
--- a/data/check-in.xlsx
+++ b/data/check-in.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="56">
   <si>
     <t xml:space="preserve">Autor: Miguel Souza Cardeal</t>
   </si>
@@ -1489,7 +1489,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="14" t="n">
         <f aca="false">Jan!C7</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" s="15" t="n">
         <f aca="false">IFERROR(E9/$E$9,"")</f>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="M9" s="15" t="n">
         <f aca="false">IFERROR(L9/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="O9" s="3"/>
     </row>
@@ -1519,7 +1519,7 @@
       <c r="D10" s="13"/>
       <c r="E10" s="14" t="n">
         <f aca="false">Jan!C8</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F10" s="15" t="n">
         <f aca="false">IFERROR(E10/$E$9,"")</f>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="M10" s="15" t="n">
         <f aca="false">IFERROR(L10/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,7 +1548,7 @@
       <c r="D11" s="13"/>
       <c r="E11" s="14" t="n">
         <f aca="false">Jan!F7</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F11" s="15" t="n">
         <f aca="false">IFERROR(E11/$E$9,"")</f>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="M11" s="15" t="n">
         <f aca="false">IFERROR(L11/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="F15" s="15" t="n">
         <f aca="false">IFERROR(E15/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="13" t="s">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="M15" s="15" t="n">
         <f aca="false">IFERROR(L15/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="F16" s="15" t="n">
         <f aca="false">IFERROR(E16/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="13" t="s">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="M16" s="15" t="n">
         <f aca="false">IFERROR(L16/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="F17" s="15" t="n">
         <f aca="false">IFERROR(E17/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="13" t="s">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="M17" s="15" t="n">
         <f aca="false">IFERROR(L17/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="F21" s="15" t="n">
         <f aca="false">IFERROR(E21/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="13" t="s">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="M21" s="15" t="n">
         <f aca="false">IFERROR(L21/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1854,7 @@
       </c>
       <c r="F22" s="15" t="n">
         <f aca="false">IFERROR(E22/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="13" t="s">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="M22" s="15" t="n">
         <f aca="false">IFERROR(L22/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="F23" s="15" t="n">
         <f aca="false">IFERROR(E23/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="13" t="s">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="M23" s="15" t="n">
         <f aca="false">IFERROR(L23/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="F27" s="15" t="n">
         <f aca="false">IFERROR(E27/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="13" t="s">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="F28" s="15" t="n">
         <f aca="false">IFERROR(E28/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="13" t="s">
@@ -2055,7 +2055,7 @@
       </c>
       <c r="M29" s="15" t="n">
         <f aca="false">IFERROR(L29/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2134,7 +2134,7 @@
       </c>
       <c r="F33" s="15" t="n">
         <f aca="false">IFERROR(E33/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="13" t="s">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="M33" s="15" t="n">
         <f aca="false">IFERROR(L33/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="O33" s="3"/>
     </row>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="F34" s="15" t="n">
         <f aca="false">IFERROR(E34/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="13" t="s">
@@ -2178,7 +2178,7 @@
       </c>
       <c r="M34" s="15" t="n">
         <f aca="false">IFERROR(L34/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="F35" s="15" t="n">
         <f aca="false">IFERROR(E35/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="13" t="s">
@@ -2207,7 +2207,7 @@
       </c>
       <c r="M35" s="15" t="n">
         <f aca="false">IFERROR(L35/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="F39" s="15" t="n">
         <f aca="false">IFERROR(E39/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="13" t="s">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="M39" s="15" t="n">
         <f aca="false">IFERROR(L39/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="F40" s="15" t="n">
         <f aca="false">IFERROR(E40/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="13" t="s">
@@ -2328,7 +2328,7 @@
       </c>
       <c r="M40" s="15" t="n">
         <f aca="false">IFERROR(L40/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="O40" s="3"/>
     </row>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="F41" s="15" t="n">
         <f aca="false">IFERROR(E41/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="13" t="s">
@@ -2358,7 +2358,7 @@
       </c>
       <c r="M41" s="15" t="n">
         <f aca="false">IFERROR(L41/$E$9,"")</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="O41" s="3"/>
     </row>
@@ -19107,7 +19107,7 @@
   <dimension ref="B1:S203"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19231,14 +19231,14 @@
       </c>
       <c r="C7" s="14" t="n">
         <f aca="false">COUNT(B:B)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="14" t="n">
         <f aca="false">COUNTIF(G:G,"Sim")</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="13" t="s">
@@ -19246,7 +19246,7 @@
       </c>
       <c r="I7" s="14" t="n">
         <f aca="false">COUNTIF(I:I,"Sim")</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -19259,14 +19259,14 @@
       </c>
       <c r="C8" s="14" t="n">
         <f aca="false">COUNT(D:D)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="14" t="n">
         <f aca="false">COUNTIF(H:H,"Sim")</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -19366,14 +19366,30 @@
       <c r="N13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+      <c r="B14" s="22" t="n">
+        <v>45725</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="23" t="n">
+        <v>5551999142035</v>
+      </c>
+      <c r="E14" s="23" t="n">
+        <v>215</v>
+      </c>
+      <c r="F14" s="22" t="n">
+        <v>45723</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -19381,14 +19397,30 @@
       <c r="N14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="B15" s="22" t="n">
+        <v>45731</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="23" t="n">
+        <v>5551999142035</v>
+      </c>
+      <c r="E15" s="23" t="n">
+        <v>215</v>
+      </c>
+      <c r="F15" s="22" t="n">
+        <v>45723</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -19396,14 +19428,30 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
+      <c r="B16" s="22" t="n">
+        <v>45792</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="23" t="n">
+        <v>5551999142035</v>
+      </c>
+      <c r="E16" s="23" t="n">
+        <v>215</v>
+      </c>
+      <c r="F16" s="22" t="n">
+        <v>45723</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -19411,14 +19459,30 @@
       <c r="N16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+      <c r="B17" s="22" t="n">
+        <v>46157</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="23" t="n">
+        <v>5551999142035</v>
+      </c>
+      <c r="E17" s="23" t="n">
+        <v>215</v>
+      </c>
+      <c r="F17" s="22" t="n">
+        <v>45723</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -19426,14 +19490,30 @@
       <c r="N17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
+      <c r="B18" s="22" t="n">
+        <v>45722</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="23" t="n">
+        <v>5551999142035</v>
+      </c>
+      <c r="E18" s="23" t="n">
+        <v>215</v>
+      </c>
+      <c r="F18" s="22" t="n">
+        <v>45723</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -19441,14 +19521,30 @@
       <c r="N18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
+      <c r="B19" s="22" t="n">
+        <v>45742</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="23" t="n">
+        <v>5551999142035</v>
+      </c>
+      <c r="E19" s="23" t="n">
+        <v>215</v>
+      </c>
+      <c r="F19" s="22" t="n">
+        <v>45723</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -19461,14 +19557,30 @@
       <c r="S19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
+      <c r="B20" s="22" t="n">
+        <v>45741</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="23" t="n">
+        <v>5551999142035</v>
+      </c>
+      <c r="E20" s="23" t="n">
+        <v>215</v>
+      </c>
+      <c r="F20" s="22" t="n">
+        <v>45723</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -19481,14 +19593,30 @@
       <c r="S20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
+      <c r="B21" s="22" t="n">
+        <v>45672</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="23" t="n">
+        <v>5551999142035</v>
+      </c>
+      <c r="E21" s="23" t="n">
+        <v>215</v>
+      </c>
+      <c r="F21" s="22" t="n">
+        <v>45723</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -19501,14 +19629,30 @@
       <c r="S21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
+      <c r="B22" s="22" t="n">
+        <v>46037</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="23" t="n">
+        <v>5551999142035</v>
+      </c>
+      <c r="E22" s="23" t="n">
+        <v>215</v>
+      </c>
+      <c r="F22" s="22" t="n">
+        <v>45723</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -22240,16 +22384,12 @@
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="G11:I11"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H14:H19" type="list">
-      <formula1>Lista!$C$3:$C$4</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G13:G19 I13:I19" type="list">
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G13:G22 I13:I22" type="list">
       <formula1>Lista!$B$3:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H13" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H13:H22" type="list">
       <formula1>Lista!$B$3:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>